<commit_message>
construyendo la clase de las validaciones de los datos de cada cliente para el envio de los correos
</commit_message>
<xml_diff>
--- a/Emails/clients/clients.xlsx
+++ b/Emails/clients/clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Promotora\rigoberto\python\process_automation\Emails\clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AA07BE6-11FF-4433-8300-B75ABAF80B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD385D1A-ECBA-4627-819F-B042931310D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4035" yWindow="3960" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -400,7 +400,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>44826</v>
+        <v>44836</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>44827</v>
+        <v>44857</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
-        <v>44828</v>
+        <v>44858</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -466,7 +466,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>44829</v>
+        <v>44859</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -480,7 +480,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>44830</v>
+        <v>44860</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
estructurando el metodo que me retorna la lista de los clientes sus correos y la fecha del envio del email
</commit_message>
<xml_diff>
--- a/Emails/clients/clients.xlsx
+++ b/Emails/clients/clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Promotora\rigoberto\python\process_automation\Emails\clients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD385D1A-ECBA-4627-819F-B042931310D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EE2EF7-3009-4A36-A445-5BB87CC33367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4035" yWindow="3960" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -36,9 +36,6 @@
     <t>correo</t>
   </si>
   <si>
-    <t>rigojmtz05+persona1@gmail.com</t>
-  </si>
-  <si>
     <t>LUIS</t>
   </si>
   <si>
@@ -70,6 +67,21 @@
   </si>
   <si>
     <t>fecha inicio del credito</t>
+  </si>
+  <si>
+    <t>rigojmtz05+persona_2@gmail.com</t>
+  </si>
+  <si>
+    <t>rigojmtz05+persona_3@gmail.com</t>
+  </si>
+  <si>
+    <t>rigojmtz05+persona_4@gmail.com</t>
+  </si>
+  <si>
+    <t>rigojmtz05+persona_5@gmail.com</t>
+  </si>
+  <si>
+    <t>rigojmtz05+persona_1@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -85,10 +97,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <family val="3"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,17 +122,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,7 +416,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +426,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -423,77 +439,84 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+      <c r="A2" s="1">
         <v>44836</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>44857</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>44858</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>44859</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>44860</v>
       </c>
       <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{8EC39522-216E-45EE-82BF-CBECDEA99A68}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{D5643451-7EA0-41B3-AB1A-E31AAC25C1F5}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{E80CB0BB-66A8-45C5-BCEA-CDE846CFAE7D}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{AE2CA595-0BDC-4BDC-9246-A8F9C669BBA9}"/>
+    <hyperlink ref="D2" r:id="rId5" xr:uid="{20451150-5494-4E1A-8174-551591731A99}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>